<commit_message>
Handle inline strings (Issue #6)
</commit_message>
<xml_diff>
--- a/Assets/Development/TestFiles/RichText.xlsx
+++ b/Assets/Development/TestFiles/RichText.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017257BB-804B-4B6A-8532-9B3A423BC9F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E83B450-53D0-41F4-9F51-1BEE5596FD31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37455" yWindow="-23850" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37755" yWindow="-24465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>Col3</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Bold Only</t>
   </si>
   <si>
     <r>
@@ -50,7 +56,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -71,14 +77,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Normal</t>
+      <t xml:space="preserve"> and plain</t>
     </r>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Bold Only</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -439,13 +439,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>